<commit_message>
More Ben Greenfield data
</commit_message>
<xml_diff>
--- a/Studies/Ketogenic Diet/Energy Output/VO2max Testing/VO2max_Others/Ben_Greenfield_VO2max/Ben_Greenfield_VO2max_Test.xlsx
+++ b/Studies/Ketogenic Diet/Energy Output/VO2max Testing/VO2max_Others/Ben_Greenfield_VO2max/Ben_Greenfield_VO2max_Test.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="25875" windowHeight="12015" activeTab="1"/>
+    <workbookView xWindow="-300" yWindow="0" windowWidth="25875" windowHeight="12015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ben_Greenfield_VO2max_Test" sheetId="1" r:id="rId1"/>
     <sheet name="FAT-CHO_VO2Percent" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1067,11 +1067,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="126101376"/>
-        <c:axId val="126061184"/>
+        <c:axId val="59217408"/>
+        <c:axId val="59219328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126101376"/>
+        <c:axId val="59217408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1083,12 +1083,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126061184"/>
+        <c:crossAx val="59219328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126061184"/>
+        <c:axId val="59219328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1100,7 +1100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126101376"/>
+        <c:crossAx val="59217408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1461,7 +1461,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>